<commit_message>
made changes to account for availability of previous years' general fund reserve data
</commit_message>
<xml_diff>
--- a/final/final_alldata_cal_sample.xlsx
+++ b/final/final_alldata_cal_sample.xlsx
@@ -811,7 +811,9 @@
       <c r="AG2" t="n">
         <v>-0.7632081709947949</v>
       </c>
-      <c r="AH2" t="inlineStr"/>
+      <c r="AH2" t="n">
+        <v>7.766967584686203</v>
+      </c>
       <c r="AI2" t="n">
         <v>6.03882861783292</v>
       </c>
@@ -837,31 +839,33 @@
       <c r="AQ2" t="n">
         <v>1.775938717539038</v>
       </c>
-      <c r="AR2" t="inlineStr"/>
+      <c r="AR2" t="n">
+        <v>8.62996398298467</v>
+      </c>
       <c r="AS2" t="n">
-        <v>8.051771490443892</v>
+        <v>6.709809575369911</v>
       </c>
       <c r="AT2" t="n">
-        <v>10.72654948822936</v>
+        <v>8.938791240191131</v>
       </c>
       <c r="AU2" t="inlineStr"/>
       <c r="AV2" t="n">
-        <v>1.12761924197352</v>
+        <v>0.9396827016445997</v>
       </c>
       <c r="AW2" t="n">
-        <v>4.612025718566799</v>
+        <v>3.843354765472333</v>
       </c>
       <c r="AX2" t="n">
-        <v>3.656826923952594</v>
+        <v>3.047355769960495</v>
       </c>
       <c r="AY2" t="n">
-        <v>11.03843137398789</v>
+        <v>9.198692811656572</v>
       </c>
       <c r="AZ2" t="n">
-        <v>1.73551174016547</v>
+        <v>1.446259783471226</v>
       </c>
       <c r="BA2" t="n">
-        <v>2.36791829005205</v>
+        <v>1.973265241710042</v>
       </c>
       <c r="BB2" t="inlineStr"/>
     </row>
@@ -2015,7 +2019,9 @@
       <c r="AG9" t="n">
         <v>0.2756134208300599</v>
       </c>
-      <c r="AH9" t="inlineStr"/>
+      <c r="AH9" t="n">
+        <v>2.489852740586195</v>
+      </c>
       <c r="AI9" t="n">
         <v>8.690715685843209</v>
       </c>
@@ -2041,31 +2047,33 @@
       <c r="AQ9" t="n">
         <v>9.567100656225449</v>
       </c>
-      <c r="AR9" t="inlineStr"/>
+      <c r="AR9" t="n">
+        <v>2.766503045095772</v>
+      </c>
       <c r="AS9" t="n">
-        <v>11.58762091445761</v>
+        <v>9.65635076204801</v>
       </c>
       <c r="AT9" t="n">
-        <v>6.137088682011059</v>
+        <v>5.11424056834255</v>
       </c>
       <c r="AU9" t="inlineStr"/>
       <c r="AV9" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AW9" t="n">
-        <v>6.666666666666666</v>
+        <v>5.555555555555555</v>
       </c>
       <c r="AX9" t="n">
-        <v>5.528778077847704</v>
+        <v>4.607315064873087</v>
       </c>
       <c r="AY9" t="n">
-        <v>11.93526552977849</v>
+        <v>9.946054608148746</v>
       </c>
       <c r="AZ9" t="n">
         <v>0</v>
       </c>
       <c r="BA9" t="n">
-        <v>12.7561342083006</v>
+        <v>10.6301118402505</v>
       </c>
       <c r="BB9" t="inlineStr"/>
     </row>
@@ -3219,7 +3227,9 @@
       <c r="AG16" t="n">
         <v>0.08234290897128597</v>
       </c>
-      <c r="AH16" t="inlineStr"/>
+      <c r="AH16" t="n">
+        <v>6.780605181657883</v>
+      </c>
       <c r="AI16" t="n">
         <v>12.81116625463111</v>
       </c>
@@ -3245,31 +3255,33 @@
       <c r="AQ16" t="n">
         <v>8.117571817284645</v>
       </c>
-      <c r="AR16" t="inlineStr"/>
+      <c r="AR16" t="n">
+        <v>7.534005757397648</v>
+      </c>
       <c r="AS16" t="n">
-        <v>17.08155500617481</v>
+        <v>14.23462917181234</v>
       </c>
       <c r="AT16" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU16" t="inlineStr"/>
       <c r="AV16" t="n">
-        <v>6.492383669322907</v>
+        <v>5.410319724435756</v>
       </c>
       <c r="AW16" t="n">
-        <v>4.993589558250893</v>
+        <v>4.161324631875744</v>
       </c>
       <c r="AX16" t="n">
-        <v>5.130489547216155</v>
+        <v>4.275407956013463</v>
       </c>
       <c r="AY16" t="n">
-        <v>12.98662802600329</v>
+        <v>10.82219002166941</v>
       </c>
       <c r="AZ16" t="n">
         <v>0</v>
       </c>
       <c r="BA16" t="n">
-        <v>10.82342908971286</v>
+        <v>9.019524241427384</v>
       </c>
       <c r="BB16" t="inlineStr"/>
     </row>
@@ -4423,7 +4435,9 @@
       <c r="AG23" t="n">
         <v>-1.117903591721056</v>
       </c>
-      <c r="AH23" t="inlineStr"/>
+      <c r="AH23" t="n">
+        <v>6.173252059861005</v>
+      </c>
       <c r="AI23" t="n">
         <v>12.89951183274062</v>
       </c>
@@ -4449,25 +4463,27 @@
       <c r="AQ23" t="n">
         <v>0</v>
       </c>
-      <c r="AR23" t="inlineStr"/>
+      <c r="AR23" t="n">
+        <v>6.859168955401117</v>
+      </c>
       <c r="AS23" t="n">
-        <v>17.19934911032082</v>
+        <v>14.33279092526735</v>
       </c>
       <c r="AT23" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU23" t="inlineStr"/>
       <c r="AV23" t="n">
-        <v>2.625006103155246</v>
+        <v>2.187505085962705</v>
       </c>
       <c r="AW23" t="n">
-        <v>4.677307112130112</v>
+        <v>3.897755926775094</v>
       </c>
       <c r="AX23" t="n">
-        <v>5.182165941865727</v>
+        <v>4.31847161822144</v>
       </c>
       <c r="AY23" t="n">
-        <v>6.799161199375036</v>
+        <v>5.665967666145864</v>
       </c>
       <c r="AZ23" t="n">
         <v>0</v>
@@ -5627,7 +5643,9 @@
       <c r="AG30" t="n">
         <v>-0.2146908392792808</v>
       </c>
-      <c r="AH30" t="inlineStr"/>
+      <c r="AH30" t="n">
+        <v>4.625516840852047</v>
+      </c>
       <c r="AI30" t="n">
         <v>5.422517457214736</v>
       </c>
@@ -5653,31 +5671,33 @@
       <c r="AQ30" t="n">
         <v>5.889818705405395</v>
       </c>
-      <c r="AR30" t="inlineStr"/>
+      <c r="AR30" t="n">
+        <v>5.139463156502274</v>
+      </c>
       <c r="AS30" t="n">
-        <v>7.230023276286315</v>
+        <v>6.025019396905263</v>
       </c>
       <c r="AT30" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU30" t="inlineStr"/>
       <c r="AV30" t="n">
-        <v>6.308047074161955</v>
+        <v>5.256705895134963</v>
       </c>
       <c r="AW30" t="n">
-        <v>5.108500218047256</v>
+        <v>4.257083515039381</v>
       </c>
       <c r="AX30" t="n">
-        <v>5.376384152189395</v>
+        <v>4.480320126824497</v>
       </c>
       <c r="AY30" t="n">
-        <v>13.04620070891509</v>
+        <v>10.87183392409591</v>
       </c>
       <c r="AZ30" t="n">
         <v>0</v>
       </c>
       <c r="BA30" t="n">
-        <v>7.853091607207192</v>
+        <v>6.544243006005995</v>
       </c>
       <c r="BB30" t="inlineStr"/>
     </row>
@@ -6831,7 +6851,9 @@
       <c r="AG37" t="n">
         <v>-0.1476164583242438</v>
       </c>
-      <c r="AH37" t="inlineStr"/>
+      <c r="AH37" t="n">
+        <v>3.803130873477562</v>
+      </c>
       <c r="AI37" t="n">
         <v>4.673611610627185</v>
       </c>
@@ -6857,31 +6879,33 @@
       <c r="AQ37" t="n">
         <v>6.392876562568172</v>
       </c>
-      <c r="AR37" t="inlineStr"/>
+      <c r="AR37" t="n">
+        <v>4.225700970530625</v>
+      </c>
       <c r="AS37" t="n">
-        <v>6.231482147502914</v>
+        <v>5.192901789585762</v>
       </c>
       <c r="AT37" t="n">
-        <v>13.02822440313514</v>
+        <v>10.85685366927928</v>
       </c>
       <c r="AU37" t="inlineStr"/>
       <c r="AV37" t="n">
-        <v>7.851048105920205</v>
+        <v>6.542540088266838</v>
       </c>
       <c r="AW37" t="n">
-        <v>5.519991653753086</v>
+        <v>4.599993044794238</v>
       </c>
       <c r="AX37" t="n">
-        <v>4.267475943851728</v>
+        <v>3.556229953209774</v>
       </c>
       <c r="AY37" t="n">
-        <v>11.50490207061041</v>
+        <v>9.587418392175344</v>
       </c>
       <c r="AZ37" t="n">
-        <v>4.452694904323698</v>
+        <v>3.710579086936415</v>
       </c>
       <c r="BA37" t="n">
-        <v>8.523835416757562</v>
+        <v>7.103196180631302</v>
       </c>
       <c r="BB37" t="inlineStr"/>
     </row>
@@ -8035,7 +8059,9 @@
       <c r="AG44" t="n">
         <v>-0.7592282369742647</v>
       </c>
-      <c r="AH44" t="inlineStr"/>
+      <c r="AH44" t="n">
+        <v>3.631761364120027</v>
+      </c>
       <c r="AI44" t="n">
         <v>9.374482864602765</v>
       </c>
@@ -8061,31 +8087,33 @@
       <c r="AQ44" t="n">
         <v>1.805788222693015</v>
       </c>
-      <c r="AR44" t="inlineStr"/>
+      <c r="AR44" t="n">
+        <v>4.035290404577808</v>
+      </c>
       <c r="AS44" t="n">
-        <v>12.49931048613702</v>
+        <v>10.41609207178085</v>
       </c>
       <c r="AT44" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU44" t="inlineStr"/>
       <c r="AV44" t="n">
-        <v>6.499833484790707</v>
+        <v>5.416527903992256</v>
       </c>
       <c r="AW44" t="n">
-        <v>5.104407029304426</v>
+        <v>4.253672524420355</v>
       </c>
       <c r="AX44" t="n">
-        <v>5.025932733163481</v>
+        <v>4.188277277636234</v>
       </c>
       <c r="AY44" t="n">
-        <v>8.900469154786835</v>
+        <v>7.41705762898903</v>
       </c>
       <c r="AZ44" t="n">
         <v>0</v>
       </c>
       <c r="BA44" t="n">
-        <v>2.407717630257353</v>
+        <v>2.006431358547794</v>
       </c>
       <c r="BB44" t="inlineStr"/>
     </row>
@@ -9239,7 +9267,9 @@
       <c r="AG51" t="n">
         <v>-0.9184897816315624</v>
       </c>
-      <c r="AH51" t="inlineStr"/>
+      <c r="AH51" t="n">
+        <v>4.417344004083851</v>
+      </c>
       <c r="AI51" t="n">
         <v>12.93358327376258</v>
       </c>
@@ -9265,31 +9295,33 @@
       <c r="AQ51" t="n">
         <v>0.6113266377632822</v>
       </c>
-      <c r="AR51" t="inlineStr"/>
+      <c r="AR51" t="n">
+        <v>4.908160004537613</v>
+      </c>
       <c r="AS51" t="n">
-        <v>17.24477769835011</v>
+        <v>14.37064808195843</v>
       </c>
       <c r="AT51" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU51" t="inlineStr"/>
       <c r="AV51" t="n">
-        <v>0.9054402908525484</v>
+        <v>0.7545335757104571</v>
       </c>
       <c r="AW51" t="n">
-        <v>4.704990873381087</v>
+        <v>3.920825727817573</v>
       </c>
       <c r="AX51" t="n">
-        <v>4.362466228884418</v>
+        <v>3.635388524070348</v>
       </c>
       <c r="AY51" t="n">
-        <v>8.395417642819652</v>
+        <v>6.996181369016377</v>
       </c>
       <c r="AZ51" t="n">
         <v>0</v>
       </c>
       <c r="BA51" t="n">
-        <v>0.8151021836843763</v>
+        <v>0.6792518197369802</v>
       </c>
       <c r="BB51" t="inlineStr"/>
     </row>
@@ -10443,7 +10475,9 @@
       <c r="AG58" t="n">
         <v>-0.2492629922697372</v>
       </c>
-      <c r="AH58" t="inlineStr"/>
+      <c r="AH58" t="n">
+        <v>2.55965188129545</v>
+      </c>
       <c r="AI58" t="n">
         <v>6.28900496282991</v>
       </c>
@@ -10469,31 +10503,33 @@
       <c r="AQ58" t="n">
         <v>5.63052755797697</v>
       </c>
-      <c r="AR58" t="inlineStr"/>
+      <c r="AR58" t="n">
+        <v>2.844057645883833</v>
+      </c>
       <c r="AS58" t="n">
-        <v>8.38533995043988</v>
+        <v>6.987783292033234</v>
       </c>
       <c r="AT58" t="n">
-        <v>11.36717601121095</v>
+        <v>9.472646676009129</v>
       </c>
       <c r="AU58" t="inlineStr"/>
       <c r="AV58" t="n">
-        <v>8.379118404223664</v>
+        <v>6.982598670186388</v>
       </c>
       <c r="AW58" t="n">
-        <v>4.986448755628341</v>
+        <v>4.155373963023617</v>
       </c>
       <c r="AX58" t="n">
-        <v>5.51282870154523</v>
+        <v>4.594023917954359</v>
       </c>
       <c r="AY58" t="n">
-        <v>11.66469471650078</v>
+        <v>9.720578930417316</v>
       </c>
       <c r="AZ58" t="n">
-        <v>1.961021401183524</v>
+        <v>1.63418450098627</v>
       </c>
       <c r="BA58" t="n">
-        <v>7.507370077302626</v>
+        <v>6.256141731085523</v>
       </c>
       <c r="BB58" t="inlineStr"/>
     </row>
@@ -11647,7 +11683,9 @@
       <c r="AG65" t="n">
         <v>-0.3991544176282017</v>
       </c>
-      <c r="AH65" t="inlineStr"/>
+      <c r="AH65" t="n">
+        <v>3.380787508484244</v>
+      </c>
       <c r="AI65" t="n">
         <v>15</v>
       </c>
@@ -11673,31 +11711,33 @@
       <c r="AQ65" t="n">
         <v>4.506341867788487</v>
       </c>
-      <c r="AR65" t="inlineStr"/>
+      <c r="AR65" t="n">
+        <v>3.756430564982494</v>
+      </c>
       <c r="AS65" t="n">
-        <v>20</v>
+        <v>16.66666666666667</v>
       </c>
       <c r="AT65" t="n">
-        <v>9.485022684223818</v>
+        <v>7.904185570186517</v>
       </c>
       <c r="AU65" t="inlineStr"/>
       <c r="AV65" t="n">
-        <v>5.171043154200968</v>
+        <v>4.309202628500807</v>
       </c>
       <c r="AW65" t="n">
-        <v>4.99593404297934</v>
+        <v>4.163278369149451</v>
       </c>
       <c r="AX65" t="n">
-        <v>4.809361211113638</v>
+        <v>4.007801009261366</v>
       </c>
       <c r="AY65" t="n">
-        <v>11.55971843346198</v>
+        <v>9.633098694551652</v>
       </c>
       <c r="AZ65" t="n">
         <v>0</v>
       </c>
       <c r="BA65" t="n">
-        <v>6.008455823717982</v>
+        <v>5.007046519764986</v>
       </c>
       <c r="BB65" t="inlineStr"/>
     </row>
@@ -12851,7 +12891,9 @@
       <c r="AG72" t="n">
         <v>0.7177140596525972</v>
       </c>
-      <c r="AH72" t="inlineStr"/>
+      <c r="AH72" t="n">
+        <v>12.68139572292896</v>
+      </c>
       <c r="AI72" t="n">
         <v>15</v>
       </c>
@@ -12877,31 +12919,33 @@
       <c r="AQ72" t="n">
         <v>12.88285544739448</v>
       </c>
-      <c r="AR72" t="inlineStr"/>
+      <c r="AR72" t="n">
+        <v>14.09043969214329</v>
+      </c>
       <c r="AS72" t="n">
-        <v>20</v>
+        <v>16.66666666666667</v>
       </c>
       <c r="AT72" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU72" t="inlineStr"/>
       <c r="AV72" t="n">
-        <v>10.88408932302568</v>
+        <v>9.070074435854732</v>
       </c>
       <c r="AW72" t="n">
-        <v>5.331957352280972</v>
+        <v>4.443297793567477</v>
       </c>
       <c r="AX72" t="n">
-        <v>5.452594356377872</v>
+        <v>4.543828630314894</v>
       </c>
       <c r="AY72" t="n">
-        <v>13.21732579224367</v>
+        <v>11.01443816020306</v>
       </c>
       <c r="AZ72" t="n">
         <v>0</v>
       </c>
       <c r="BA72" t="n">
-        <v>17.17714059652597</v>
+        <v>14.31428383043831</v>
       </c>
       <c r="BB72" t="inlineStr"/>
     </row>
@@ -14055,7 +14099,9 @@
       <c r="AG79" t="n">
         <v>0.2100908725708175</v>
       </c>
-      <c r="AH79" t="inlineStr"/>
+      <c r="AH79" t="n">
+        <v>10.89093027564838</v>
+      </c>
       <c r="AI79" t="n">
         <v>14.09108823343128</v>
       </c>
@@ -14081,31 +14127,33 @@
       <c r="AQ79" t="n">
         <v>9.075681544281132</v>
       </c>
-      <c r="AR79" t="inlineStr"/>
+      <c r="AR79" t="n">
+        <v>12.10103363960931</v>
+      </c>
       <c r="AS79" t="n">
-        <v>18.78811764457504</v>
+        <v>15.65676470381253</v>
       </c>
       <c r="AT79" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU79" t="inlineStr"/>
       <c r="AV79" t="n">
-        <v>11.75890553317023</v>
+        <v>9.799087944308527</v>
       </c>
       <c r="AW79" t="n">
-        <v>5.235842773675601</v>
+        <v>4.363202311396335</v>
       </c>
       <c r="AX79" t="n">
-        <v>6.120088805386379</v>
+        <v>5.10007400448865</v>
       </c>
       <c r="AY79" t="n">
-        <v>13.25160514434062</v>
+        <v>11.04300428695052</v>
       </c>
       <c r="AZ79" t="n">
-        <v>6.074919618015043</v>
+        <v>5.062433015012537</v>
       </c>
       <c r="BA79" t="n">
-        <v>12.10090872570817</v>
+        <v>10.08409060475681</v>
       </c>
       <c r="BB79" t="inlineStr"/>
     </row>
@@ -15259,7 +15307,9 @@
       <c r="AG86" t="n">
         <v>-0.5190948239248201</v>
       </c>
-      <c r="AH86" t="inlineStr"/>
+      <c r="AH86" t="n">
+        <v>7.035984066127872</v>
+      </c>
       <c r="AI86" t="n">
         <v>14.19269023906631</v>
       </c>
@@ -15285,31 +15335,33 @@
       <c r="AQ86" t="n">
         <v>3.606788820563849</v>
       </c>
-      <c r="AR86" t="inlineStr"/>
+      <c r="AR86" t="n">
+        <v>7.817760073475414</v>
+      </c>
       <c r="AS86" t="n">
-        <v>18.92358698542174</v>
+        <v>15.76965582118479</v>
       </c>
       <c r="AT86" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU86" t="inlineStr"/>
       <c r="AV86" t="n">
-        <v>3.37003678435023</v>
+        <v>2.808363986958525</v>
       </c>
       <c r="AW86" t="n">
-        <v>4.92124294962337</v>
+        <v>4.101035791352809</v>
       </c>
       <c r="AX86" t="n">
-        <v>4.650104950418568</v>
+        <v>3.87508745868214</v>
       </c>
       <c r="AY86" t="n">
-        <v>12.49342392153194</v>
+        <v>10.41118660127662</v>
       </c>
       <c r="AZ86" t="n">
         <v>0</v>
       </c>
       <c r="BA86" t="n">
-        <v>4.809051760751799</v>
+        <v>4.007543133959833</v>
       </c>
       <c r="BB86" t="inlineStr"/>
     </row>
@@ -16463,7 +16515,9 @@
       <c r="AG93" t="n">
         <v>0.2679144497637393</v>
       </c>
-      <c r="AH93" t="inlineStr"/>
+      <c r="AH93" t="n">
+        <v>15</v>
+      </c>
       <c r="AI93" t="n">
         <v>15</v>
       </c>
@@ -16489,31 +16543,33 @@
       <c r="AQ93" t="n">
         <v>9.509358373228045</v>
       </c>
-      <c r="AR93" t="inlineStr"/>
+      <c r="AR93" t="n">
+        <v>16.66666666666667</v>
+      </c>
       <c r="AS93" t="n">
-        <v>20</v>
+        <v>16.66666666666667</v>
       </c>
       <c r="AT93" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU93" t="inlineStr"/>
       <c r="AV93" t="n">
-        <v>10.973715286694</v>
+        <v>9.14476273891167</v>
       </c>
       <c r="AW93" t="n">
-        <v>4.880974056610098</v>
+        <v>4.067478380508415</v>
       </c>
       <c r="AX93" t="n">
-        <v>6.195701344428919</v>
+        <v>5.163084453690766</v>
       </c>
       <c r="AY93" t="n">
-        <v>10.94642904847501</v>
+        <v>9.122024207062505</v>
       </c>
       <c r="AZ93" t="n">
         <v>0</v>
       </c>
       <c r="BA93" t="n">
-        <v>12.67914449763739</v>
+        <v>10.56595374803116</v>
       </c>
       <c r="BB93" t="inlineStr"/>
     </row>
@@ -17667,7 +17723,9 @@
       <c r="AG100" t="n">
         <v>0.2452416175534901</v>
       </c>
-      <c r="AH100" t="inlineStr"/>
+      <c r="AH100" t="n">
+        <v>6.764836722196551</v>
+      </c>
       <c r="AI100" t="n">
         <v>9.607536774415717</v>
       </c>
@@ -17693,31 +17751,33 @@
       <c r="AQ100" t="n">
         <v>9.339312131651177</v>
       </c>
-      <c r="AR100" t="inlineStr"/>
+      <c r="AR100" t="n">
+        <v>7.516485246885058</v>
+      </c>
       <c r="AS100" t="n">
-        <v>12.81004903255429</v>
+        <v>10.67504086046191</v>
       </c>
       <c r="AT100" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU100" t="inlineStr"/>
       <c r="AV100" t="n">
-        <v>8.215319616672884</v>
+        <v>6.846099680560738</v>
       </c>
       <c r="AW100" t="n">
-        <v>4.551671542405035</v>
+        <v>3.793059618670863</v>
       </c>
       <c r="AX100" t="n">
-        <v>5.149873721453028</v>
+        <v>4.291561434544191</v>
       </c>
       <c r="AY100" t="n">
-        <v>10.24577214921015</v>
+        <v>8.538143457675126</v>
       </c>
       <c r="AZ100" t="n">
-        <v>1.739037779697147</v>
+        <v>1.449198149747623</v>
       </c>
       <c r="BA100" t="n">
-        <v>12.4524161755349</v>
+        <v>10.37701347961242</v>
       </c>
       <c r="BB100" t="inlineStr"/>
     </row>
@@ -18871,7 +18931,9 @@
       <c r="AG107" t="n">
         <v>-0.1585581322425912</v>
       </c>
-      <c r="AH107" t="inlineStr"/>
+      <c r="AH107" t="n">
+        <v>3.27837300365398</v>
+      </c>
       <c r="AI107" t="n">
         <v>11.67317088734987</v>
       </c>
@@ -18897,31 +18959,33 @@
       <c r="AQ107" t="n">
         <v>6.310814008180566</v>
       </c>
-      <c r="AR107" t="inlineStr"/>
+      <c r="AR107" t="n">
+        <v>3.642636670726645</v>
+      </c>
       <c r="AS107" t="n">
-        <v>15.56422784979983</v>
+        <v>12.97018987483319</v>
       </c>
       <c r="AT107" t="n">
-        <v>8.663216611104858</v>
+        <v>7.219347175920715</v>
       </c>
       <c r="AU107" t="inlineStr"/>
       <c r="AV107" t="n">
-        <v>6.631367652427682</v>
+        <v>5.526139710356402</v>
       </c>
       <c r="AW107" t="n">
-        <v>4.557975684143914</v>
+        <v>3.798313070119929</v>
       </c>
       <c r="AX107" t="n">
-        <v>4.725079397419045</v>
+        <v>3.937566164515871</v>
       </c>
       <c r="AY107" t="n">
-        <v>7.639305815676953</v>
+        <v>6.366088179730794</v>
       </c>
       <c r="AZ107" t="n">
-        <v>0.2486201068170937</v>
+        <v>0.2071834223475781</v>
       </c>
       <c r="BA107" t="n">
-        <v>8.414418677574087</v>
+        <v>7.012015564645074</v>
       </c>
       <c r="BB107" t="inlineStr"/>
     </row>
@@ -20075,7 +20139,9 @@
       <c r="AG114" t="n">
         <v>-0.6611288485321232</v>
       </c>
-      <c r="AH114" t="inlineStr"/>
+      <c r="AH114" t="n">
+        <v>14.77090003467754</v>
+      </c>
       <c r="AI114" t="n">
         <v>8.852224645550253</v>
       </c>
@@ -20101,31 +20167,33 @@
       <c r="AQ114" t="n">
         <v>2.541533636009076</v>
       </c>
-      <c r="AR114" t="inlineStr"/>
+      <c r="AR114" t="n">
+        <v>16.41211114964171</v>
+      </c>
       <c r="AS114" t="n">
-        <v>11.802966194067</v>
+        <v>9.835805161722504</v>
       </c>
       <c r="AT114" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU114" t="inlineStr"/>
       <c r="AV114" t="n">
-        <v>6.28865024155471</v>
+        <v>5.240541867962259</v>
       </c>
       <c r="AW114" t="n">
-        <v>4.771320708484081</v>
+        <v>3.976100590403401</v>
       </c>
       <c r="AX114" t="n">
-        <v>4.945649326785484</v>
+        <v>4.121374438987903</v>
       </c>
       <c r="AY114" t="n">
-        <v>11.61049463268329</v>
+        <v>9.675412193902746</v>
       </c>
       <c r="AZ114" t="n">
-        <v>2.163536423632734</v>
+        <v>1.802947019693945</v>
       </c>
       <c r="BA114" t="n">
-        <v>3.388711514678768</v>
+        <v>2.823926262232307</v>
       </c>
       <c r="BB114" t="inlineStr"/>
     </row>
@@ -21279,7 +21347,9 @@
       <c r="AG121" t="n">
         <v>-0.4040907357804576</v>
       </c>
-      <c r="AH121" t="inlineStr"/>
+      <c r="AH121" t="n">
+        <v>4.138920410960259</v>
+      </c>
       <c r="AI121" t="n">
         <v>13.49961220275747</v>
       </c>
@@ -21305,31 +21375,33 @@
       <c r="AQ121" t="n">
         <v>4.469319481646568</v>
       </c>
-      <c r="AR121" t="inlineStr"/>
+      <c r="AR121" t="n">
+        <v>4.59880045662251</v>
+      </c>
       <c r="AS121" t="n">
-        <v>17.99948293700996</v>
+        <v>14.99956911417497</v>
       </c>
       <c r="AT121" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU121" t="inlineStr"/>
       <c r="AV121" t="n">
-        <v>4.792929300986497</v>
+        <v>3.994107750822081</v>
       </c>
       <c r="AW121" t="n">
-        <v>4.835586871321276</v>
+        <v>4.029655726101064</v>
       </c>
       <c r="AX121" t="n">
-        <v>4.336116468748709</v>
+        <v>3.613430390623924</v>
       </c>
       <c r="AY121" t="n">
-        <v>12.88456428048389</v>
+        <v>10.73713690040325</v>
       </c>
       <c r="AZ121" t="n">
         <v>0</v>
       </c>
       <c r="BA121" t="n">
-        <v>5.959092642195424</v>
+        <v>4.965910535162854</v>
       </c>
       <c r="BB121" t="inlineStr"/>
     </row>
@@ -22483,7 +22555,9 @@
       <c r="AG128" t="n">
         <v>0.1436319120163013</v>
       </c>
-      <c r="AH128" t="inlineStr"/>
+      <c r="AH128" t="n">
+        <v>11.67889726189139</v>
+      </c>
       <c r="AI128" t="n">
         <v>14.52481984714908</v>
       </c>
@@ -22509,31 +22583,33 @@
       <c r="AQ128" t="n">
         <v>8.57723934012226</v>
       </c>
-      <c r="AR128" t="inlineStr"/>
+      <c r="AR128" t="n">
+        <v>12.97655251321265</v>
+      </c>
       <c r="AS128" t="n">
-        <v>19.36642646286543</v>
+        <v>16.13868871905453</v>
       </c>
       <c r="AT128" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU128" t="inlineStr"/>
       <c r="AV128" t="n">
-        <v>10.13083021430367</v>
+        <v>8.442358511919725</v>
       </c>
       <c r="AW128" t="n">
-        <v>5.263871041889214</v>
+        <v>4.386559201574345</v>
       </c>
       <c r="AX128" t="n">
-        <v>5.419032130095893</v>
+        <v>4.515860108413245</v>
       </c>
       <c r="AY128" t="n">
-        <v>13.13306638427871</v>
+        <v>10.94422198689893</v>
       </c>
       <c r="AZ128" t="n">
         <v>0</v>
       </c>
       <c r="BA128" t="n">
-        <v>11.43631912016301</v>
+        <v>9.530265933469177</v>
       </c>
       <c r="BB128" t="inlineStr"/>
     </row>
@@ -23687,7 +23763,9 @@
       <c r="AG135" t="n">
         <v>-0.01456775803574643</v>
       </c>
-      <c r="AH135" t="inlineStr"/>
+      <c r="AH135" t="n">
+        <v>11.25328899616736</v>
+      </c>
       <c r="AI135" t="n">
         <v>12.84028894774634</v>
       </c>
@@ -23713,31 +23791,33 @@
       <c r="AQ135" t="n">
         <v>7.390741814731902</v>
       </c>
-      <c r="AR135" t="inlineStr"/>
+      <c r="AR135" t="n">
+        <v>12.50365444018596</v>
+      </c>
       <c r="AS135" t="n">
-        <v>17.12038526366178</v>
+        <v>14.26698771971815</v>
       </c>
       <c r="AT135" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU135" t="inlineStr"/>
       <c r="AV135" t="n">
-        <v>6.351606296736254</v>
+        <v>5.293005247280211</v>
       </c>
       <c r="AW135" t="n">
-        <v>4.674898666504088</v>
+        <v>3.895748888753408</v>
       </c>
       <c r="AX135" t="n">
-        <v>4.837782651515295</v>
+        <v>4.031485542929413</v>
       </c>
       <c r="AY135" t="n">
-        <v>12.59122049056134</v>
+        <v>10.49268374213445</v>
       </c>
       <c r="AZ135" t="n">
-        <v>0.5881555245929579</v>
+        <v>0.490129603827465</v>
       </c>
       <c r="BA135" t="n">
-        <v>9.854322419642536</v>
+        <v>8.211935349702113</v>
       </c>
       <c r="BB135" t="inlineStr"/>
     </row>
@@ -24891,7 +24971,9 @@
       <c r="AG142" t="n">
         <v>-0.159854430260688</v>
       </c>
-      <c r="AH142" t="inlineStr"/>
+      <c r="AH142" t="n">
+        <v>15</v>
+      </c>
       <c r="AI142" t="n">
         <v>8.545783952406545</v>
       </c>
@@ -24917,31 +24999,33 @@
       <c r="AQ142" t="n">
         <v>6.30109177304484</v>
       </c>
-      <c r="AR142" t="inlineStr"/>
+      <c r="AR142" t="n">
+        <v>16.66666666666667</v>
+      </c>
       <c r="AS142" t="n">
-        <v>11.39437860320873</v>
+        <v>9.49531550267394</v>
       </c>
       <c r="AT142" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU142" t="inlineStr"/>
       <c r="AV142" t="n">
-        <v>8.757390142172101</v>
+        <v>7.297825118476752</v>
       </c>
       <c r="AW142" t="n">
-        <v>4.546612623157269</v>
+        <v>3.788843852631058</v>
       </c>
       <c r="AX142" t="n">
-        <v>5.534358897972081</v>
+        <v>4.611965748310068</v>
       </c>
       <c r="AY142" t="n">
-        <v>13.01039444410205</v>
+        <v>10.84199537008505</v>
       </c>
       <c r="AZ142" t="n">
-        <v>2.095274778598537</v>
+        <v>1.746062315498781</v>
       </c>
       <c r="BA142" t="n">
-        <v>8.40145569739312</v>
+        <v>7.001213081160934</v>
       </c>
       <c r="BB142" t="inlineStr"/>
     </row>
@@ -26095,7 +26179,9 @@
       <c r="AG149" t="n">
         <v>-0.02914406051933791</v>
       </c>
-      <c r="AH149" t="inlineStr"/>
+      <c r="AH149" t="n">
+        <v>15</v>
+      </c>
       <c r="AI149" t="n">
         <v>15</v>
       </c>
@@ -26121,31 +26207,33 @@
       <c r="AQ149" t="n">
         <v>7.281419546104965</v>
       </c>
-      <c r="AR149" t="inlineStr"/>
+      <c r="AR149" t="n">
+        <v>16.66666666666667</v>
+      </c>
       <c r="AS149" t="n">
-        <v>20</v>
+        <v>16.66666666666667</v>
       </c>
       <c r="AT149" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU149" t="inlineStr"/>
       <c r="AV149" t="n">
-        <v>6.80667467011207</v>
+        <v>5.672228891760058</v>
       </c>
       <c r="AW149" t="n">
-        <v>4.837677055490607</v>
+        <v>4.031397546242173</v>
       </c>
       <c r="AX149" t="n">
-        <v>4.946912541620055</v>
+        <v>4.122427118016713</v>
       </c>
       <c r="AY149" t="n">
-        <v>11.82081070108584</v>
+        <v>9.8506755842382</v>
       </c>
       <c r="AZ149" t="n">
-        <v>3.102032541146488</v>
+        <v>2.585027117622074</v>
       </c>
       <c r="BA149" t="n">
-        <v>9.70855939480662</v>
+        <v>8.090466162338851</v>
       </c>
       <c r="BB149" t="inlineStr"/>
     </row>
@@ -27299,7 +27387,9 @@
       <c r="AG156" t="n">
         <v>-0.2291109981853156</v>
       </c>
-      <c r="AH156" t="inlineStr"/>
+      <c r="AH156" t="n">
+        <v>4.971714977712679</v>
+      </c>
       <c r="AI156" t="n">
         <v>10.3932262366326</v>
       </c>
@@ -27325,31 +27415,33 @@
       <c r="AQ156" t="n">
         <v>5.781667513610133</v>
       </c>
-      <c r="AR156" t="inlineStr"/>
+      <c r="AR156" t="n">
+        <v>5.524127753014088</v>
+      </c>
       <c r="AS156" t="n">
-        <v>13.8576349821768</v>
+        <v>11.548029151814</v>
       </c>
       <c r="AT156" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU156" t="inlineStr"/>
       <c r="AV156" t="n">
-        <v>5.826910563198377</v>
+        <v>4.855758802665314</v>
       </c>
       <c r="AW156" t="n">
-        <v>4.530597152925147</v>
+        <v>3.775497627437623</v>
       </c>
       <c r="AX156" t="n">
-        <v>4.73981987436707</v>
+        <v>3.949849895305892</v>
       </c>
       <c r="AY156" t="n">
-        <v>9.947353963922328</v>
+        <v>8.289461636601942</v>
       </c>
       <c r="AZ156" t="n">
-        <v>0.00649772598942999</v>
+        <v>0.005414771657858326</v>
       </c>
       <c r="BA156" t="n">
-        <v>7.708890018146843</v>
+        <v>6.42407501512237</v>
       </c>
       <c r="BB156" t="inlineStr"/>
     </row>
@@ -28503,7 +28595,9 @@
       <c r="AG163" t="n">
         <v>-0.1561799361143665</v>
       </c>
-      <c r="AH163" t="inlineStr"/>
+      <c r="AH163" t="n">
+        <v>5.5179764543646</v>
+      </c>
       <c r="AI163" t="n">
         <v>12.53045709879922</v>
       </c>
@@ -28529,31 +28623,33 @@
       <c r="AQ163" t="n">
         <v>6.328650479142252</v>
       </c>
-      <c r="AR163" t="inlineStr"/>
+      <c r="AR163" t="n">
+        <v>6.131084949294</v>
+      </c>
       <c r="AS163" t="n">
-        <v>16.70727613173229</v>
+        <v>13.92273010977691</v>
       </c>
       <c r="AT163" t="n">
-        <v>13.33333333333333</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="AU163" t="inlineStr"/>
       <c r="AV163" t="n">
-        <v>7.953055235123779</v>
+        <v>6.627546029269817</v>
       </c>
       <c r="AW163" t="n">
-        <v>5.04983919581306</v>
+        <v>4.208199329844217</v>
       </c>
       <c r="AX163" t="n">
-        <v>5.440017317278546</v>
+        <v>4.533347764398789</v>
       </c>
       <c r="AY163" t="n">
-        <v>13.16272852930618</v>
+        <v>10.96894044108848</v>
       </c>
       <c r="AZ163" t="n">
         <v>0</v>
       </c>
       <c r="BA163" t="n">
-        <v>8.438200638856335</v>
+        <v>7.031833865713613</v>
       </c>
       <c r="BB163" t="inlineStr"/>
     </row>
@@ -29707,7 +29803,9 @@
       <c r="AG170" t="n">
         <v>-0.4058451924700272</v>
       </c>
-      <c r="AH170" t="inlineStr"/>
+      <c r="AH170" t="n">
+        <v>5.22188076308243</v>
+      </c>
       <c r="AI170" t="n">
         <v>9.087491650569703</v>
       </c>
@@ -29733,31 +29831,33 @@
       <c r="AQ170" t="n">
         <v>4.456161056474796</v>
       </c>
-      <c r="AR170" t="inlineStr"/>
+      <c r="AR170" t="n">
+        <v>5.802089736758256</v>
+      </c>
       <c r="AS170" t="n">
-        <v>12.11665553409294</v>
+        <v>10.09721294507745</v>
       </c>
       <c r="AT170" t="n">
-        <v>9.290899566454112</v>
+        <v>7.742416305378428</v>
       </c>
       <c r="AU170" t="inlineStr"/>
       <c r="AV170" t="n">
-        <v>6.729922626946539</v>
+        <v>5.608268855788783</v>
       </c>
       <c r="AW170" t="n">
-        <v>5.004346613376535</v>
+        <v>4.170288844480447</v>
       </c>
       <c r="AX170" t="n">
-        <v>4.659349057152604</v>
+        <v>3.882790880960504</v>
       </c>
       <c r="AY170" t="n">
-        <v>12.61528073248606</v>
+        <v>10.51273394373838</v>
       </c>
       <c r="AZ170" t="n">
         <v>0</v>
       </c>
       <c r="BA170" t="n">
-        <v>5.941548075299728</v>
+        <v>4.951290062749774</v>
       </c>
       <c r="BB170" t="inlineStr"/>
     </row>

</xml_diff>